<commit_message>
Revert "Merge branch 'master' of https://github.com/anodiamadm/Docs"
This reverts commit 359e83d67a17642d7c501f9390a8045eb61f7eb8, reversing
changes made to 3ef48aefceaa73ed30a9e2e5bb29e512807ac384.
</commit_message>
<xml_diff>
--- a/AgilePM/ProductBacklog.xlsx
+++ b/AgilePM/ProductBacklog.xlsx
@@ -471,7 +471,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="259">
   <si>
     <t>Anodiam</t>
   </si>
@@ -3244,6 +3244,30 @@
   </si>
   <si>
     <r>
+      <t>visit the Signup / Login page at the link anodiam.com/teacher, key in my valid user id and password and click on the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Login button</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+  </si>
+  <si>
+    <r>
       <rPr>
         <b/>
         <sz val="10"/>
@@ -4010,7 +4034,91 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Click on the Forgot Password / Change Password link </t>
+    <r>
+      <t>As a(intending to login)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>user</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">of Anodiam </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>teacher app</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">visit the Signup / Login page at the link anodiam.com/teacher, get an option to create new password if forgotton and redirected to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>login page</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
   </si>
   <si>
     <r>
@@ -4024,7 +4132,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> Change Password in the Teacher App</t>
+      <t xml:space="preserve"> Change Password </t>
     </r>
   </si>
   <si>
@@ -4045,17 +4153,17 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> I have clicked on the forgotton / chage my password link in </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>my Valid Email Id</t>
+      <t xml:space="preserve"> I have forgotton or want to chage my password in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Teacher Login page</t>
     </r>
     <r>
       <rPr>
@@ -4084,6 +4192,104 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve"> I click on "Forgot Password" button in Anodiam Teacher App
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I shall be able to receive an Email in my valid Emai Id containing the link to go to Change/Forgot Password page in Teacher App.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on the Forgot Password / Change Password link </t>
+  </si>
+  <si>
+    <r>
+      <t>I shall be able to</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Change Password in the Teacher App</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I have clicked on the forgotton / chage my password link in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>my Valid Email Id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve"> I click on "Forgot Password / Change Password" link in my valid Emai id
 </t>
     </r>
@@ -4478,229 +4684,6 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> I shall be able to create a New Password  in the Teacher App.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>visit the Signup / Login page at anodiam.com/teacher, key in my valid user id and password and click on the</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Login button</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>visit the Signup / Login page at anodiam.com/teacher, and find a link to create new password</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Unsigned user with forgotton password of</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Anodiam </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>teacher app</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">I shall be able to click the link and visit the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Forget Password</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> page</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> I shall be able to receive an Email in my valid Emai Id containing the link to go to Change/Forgot Password page in Teacher App.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Given</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> I have forgotton my password for Anodiam </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Teacher</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> app
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>When</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> I click on </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Forgot Password</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> link in Anodiam Teacher app, Login / Signup page
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Then</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> I shall be able to visit the Forget Password page</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">visit the Forget Password page, fill  up the required verification details and click on the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Send Password</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> button</t>
     </r>
   </si>
 </sst>
@@ -4999,7 +4982,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5162,7 +5145,6 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -5448,31 +5430,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="60" x14ac:dyDescent="0.2">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -5669,11 +5651,11 @@
       <c r="C3" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="79" t="s">
+      <c r="D3" s="78" t="s">
         <v>174</v>
       </c>
-      <c r="E3" s="80"/>
-      <c r="F3" s="81"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="80"/>
       <c r="G3" s="56"/>
       <c r="H3" s="42" t="s">
         <v>185</v>
@@ -5745,11 +5727,11 @@
       <c r="C5" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="79" t="s">
+      <c r="D5" s="78" t="s">
         <v>175</v>
       </c>
-      <c r="E5" s="80"/>
-      <c r="F5" s="81"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="80"/>
       <c r="G5" s="56"/>
       <c r="H5" s="36"/>
       <c r="I5" s="36">
@@ -5817,11 +5799,11 @@
       <c r="C7" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="82" t="s">
+      <c r="D7" s="81" t="s">
         <v>176</v>
       </c>
-      <c r="E7" s="83"/>
-      <c r="F7" s="84"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="83"/>
       <c r="G7" s="59" t="s">
         <v>178</v>
       </c>
@@ -5963,11 +5945,11 @@
       <c r="C11" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="76" t="s">
+      <c r="D11" s="75" t="s">
         <v>159</v>
       </c>
-      <c r="E11" s="77"/>
-      <c r="F11" s="78"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="77"/>
       <c r="G11" s="36" t="s">
         <v>161</v>
       </c>
@@ -5997,11 +5979,11 @@
       <c r="C12" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="76" t="s">
+      <c r="D12" s="75" t="s">
         <v>160</v>
       </c>
-      <c r="E12" s="77"/>
-      <c r="F12" s="78"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="77"/>
       <c r="G12" s="36" t="s">
         <v>162</v>
       </c>
@@ -6123,11 +6105,11 @@
       <c r="C16" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="73" t="s">
+      <c r="D16" s="72" t="s">
         <v>206</v>
       </c>
-      <c r="E16" s="74"/>
-      <c r="F16" s="75"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="74"/>
       <c r="G16" s="62" t="s">
         <v>191</v>
       </c>
@@ -8104,13 +8086,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M507"/>
+  <dimension ref="A1:M506"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="G15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8227,7 +8209,7 @@
         <v>190</v>
       </c>
       <c r="G3" s="36" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H3" s="42" t="s">
         <v>215</v>
@@ -8262,7 +8244,7 @@
         <v>199</v>
       </c>
       <c r="F4" s="36" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G4" s="36" t="s">
         <v>218</v>
@@ -8288,11 +8270,11 @@
       <c r="C5" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="76" t="s">
+      <c r="D5" s="75" t="s">
         <v>206</v>
       </c>
-      <c r="E5" s="77"/>
-      <c r="F5" s="78"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="77"/>
       <c r="G5" s="36" t="s">
         <v>191</v>
       </c>
@@ -8450,10 +8432,10 @@
         <v>222</v>
       </c>
       <c r="F10" s="36" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G10" s="36" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="H10" s="36"/>
       <c r="I10" s="36"/>
@@ -8478,13 +8460,13 @@
         <v>225</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>254</v>
+        <v>226</v>
       </c>
       <c r="F11" s="36" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G11" s="36" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H11" s="42"/>
       <c r="I11" s="36"/>
@@ -8492,7 +8474,7 @@
         <v>5</v>
       </c>
       <c r="K11" s="43">
-        <f t="shared" ref="K11:K19" si="0">IF(I11=0,0,J11/I11)</f>
+        <f t="shared" ref="K11:K18" si="0">IF(I11=0,0,J11/I11)</f>
         <v>0</v>
       </c>
       <c r="L11" s="36"/>
@@ -8509,20 +8491,18 @@
         <v>19</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="E12" s="36" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="G12" s="36" t="s">
-        <v>259</v>
-      </c>
-      <c r="H12" s="42" t="s">
-        <v>258</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="H12" s="42"/>
       <c r="I12" s="36"/>
       <c r="J12" s="40">
         <v>5</v>
@@ -8534,34 +8514,43 @@
       <c r="L12" s="36"/>
       <c r="M12" s="35"/>
     </row>
-    <row r="13" spans="1:13" s="67" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" s="66" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="35">
         <v>12</v>
       </c>
       <c r="B13" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="36" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E13" s="36" t="s">
-        <v>260</v>
-      </c>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
+        <v>247</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>248</v>
+      </c>
+      <c r="G13" s="36" t="s">
+        <v>249</v>
+      </c>
       <c r="H13" s="42"/>
       <c r="I13" s="36"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="43"/>
+      <c r="J13" s="40">
+        <v>5</v>
+      </c>
+      <c r="K13" s="43">
+        <f t="shared" ref="K13" si="2">IF(I13=0,0,J13/I13)</f>
+        <v>0</v>
+      </c>
       <c r="L13" s="36"/>
       <c r="M13" s="35"/>
     </row>
     <row r="14" spans="1:13" s="66" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="35">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="35" t="s">
         <v>17</v>
@@ -8570,16 +8559,16 @@
         <v>19</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="E14" s="36" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="F14" s="36" t="s">
-        <v>243</v>
+        <v>255</v>
       </c>
       <c r="G14" s="36" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="H14" s="42"/>
       <c r="I14" s="36"/>
@@ -8587,7 +8576,7 @@
         <v>5</v>
       </c>
       <c r="K14" s="43">
-        <f t="shared" ref="K14" si="2">IF(I14=0,0,J14/I14)</f>
+        <f t="shared" ref="K14" si="3">IF(I14=0,0,J14/I14)</f>
         <v>0</v>
       </c>
       <c r="L14" s="36"/>
@@ -8595,7 +8584,7 @@
     </row>
     <row r="15" spans="1:13" s="66" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="35">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="35" t="s">
         <v>17</v>
@@ -8604,16 +8593,16 @@
         <v>19</v>
       </c>
       <c r="D15" s="36" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="E15" s="36" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="G15" s="36" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="H15" s="42"/>
       <c r="I15" s="36"/>
@@ -8621,49 +8610,46 @@
         <v>5</v>
       </c>
       <c r="K15" s="43">
-        <f t="shared" ref="K15" si="3">IF(I15=0,0,J15/I15)</f>
+        <f t="shared" ref="K15" si="4">IF(I15=0,0,J15/I15)</f>
         <v>0</v>
       </c>
       <c r="L15" s="36"/>
       <c r="M15" s="35"/>
     </row>
-    <row r="16" spans="1:13" s="66" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" s="65" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="35">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="35" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="36" t="s">
-        <v>249</v>
+        <v>180</v>
       </c>
       <c r="E16" s="36" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="F16" s="36" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="G16" s="36" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="H16" s="42"/>
       <c r="I16" s="36"/>
       <c r="J16" s="40">
         <v>5</v>
       </c>
-      <c r="K16" s="43">
-        <f t="shared" ref="K16" si="4">IF(I16=0,0,J16/I16)</f>
-        <v>0</v>
-      </c>
+      <c r="K16" s="43"/>
       <c r="L16" s="36"/>
       <c r="M16" s="35"/>
     </row>
-    <row r="17" spans="1:13" s="65" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="35">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="35" t="s">
         <v>17</v>
@@ -8675,13 +8661,13 @@
         <v>180</v>
       </c>
       <c r="E17" s="36" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F17" s="36" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G17" s="36" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="H17" s="42"/>
       <c r="I17" s="36"/>
@@ -8692,9 +8678,9 @@
       <c r="L17" s="36"/>
       <c r="M17" s="35"/>
     </row>
-    <row r="18" spans="1:13" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="35">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="35" t="s">
         <v>17</v>
@@ -8706,41 +8692,44 @@
         <v>180</v>
       </c>
       <c r="E18" s="36" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F18" s="36" t="s">
         <v>238</v>
       </c>
       <c r="G18" s="36" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H18" s="42"/>
       <c r="I18" s="36"/>
       <c r="J18" s="40">
         <v>5</v>
       </c>
-      <c r="K18" s="43"/>
+      <c r="K18" s="43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L18" s="36"/>
       <c r="M18" s="35"/>
     </row>
-    <row r="19" spans="1:13" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="35">
+        <v>18</v>
+      </c>
+      <c r="B19" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="36" t="s">
         <v>19</v>
       </c>
       <c r="D19" s="36" t="s">
         <v>180</v>
       </c>
       <c r="E19" s="36" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F19" s="36" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="G19" s="36" t="s">
         <v>232</v>
@@ -8750,40 +8739,21 @@
       <c r="J19" s="40">
         <v>5</v>
       </c>
-      <c r="K19" s="43">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="K19" s="43"/>
       <c r="L19" s="36"/>
       <c r="M19" s="35"/>
     </row>
-    <row r="20" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A20" s="35">
-        <v>18</v>
-      </c>
-      <c r="B20" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="E20" s="36" t="s">
-        <v>230</v>
-      </c>
-      <c r="F20" s="36" t="s">
-        <v>229</v>
-      </c>
-      <c r="G20" s="36" t="s">
-        <v>231</v>
-      </c>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="35"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
       <c r="H20" s="42"/>
       <c r="I20" s="36"/>
-      <c r="J20" s="40">
-        <v>5</v>
-      </c>
+      <c r="J20" s="40"/>
       <c r="K20" s="43"/>
       <c r="L20" s="36"/>
       <c r="M20" s="35"/>
@@ -16078,39 +16048,24 @@
       <c r="L506" s="36"/>
       <c r="M506" s="35"/>
     </row>
-    <row r="507" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A507" s="35"/>
-      <c r="B507" s="36"/>
-      <c r="C507" s="36"/>
-      <c r="D507" s="36"/>
-      <c r="E507" s="36"/>
-      <c r="F507" s="36"/>
-      <c r="G507" s="36"/>
-      <c r="H507" s="42"/>
-      <c r="I507" s="36"/>
-      <c r="J507" s="40"/>
-      <c r="K507" s="43"/>
-      <c r="L507" s="36"/>
-      <c r="M507" s="35"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D5:F5"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Business Value Error!" error="Business Value should be an integer between 1 to 5!" sqref="J2:J507">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Business Value Error!" error="Business Value should be an integer between 1 to 5!" sqref="J2:J506">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C507">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C506">
       <formula1>"Epic,Story"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B507">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B506">
       <formula1>"Feature,Enabler"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Estimates Error!" error="Enter Story Points in Fibonacci!!!" promptTitle="Enter Story Points in Fibonacci" prompt="Enter Story Points in Fibonacci Series: 1, 2, 3, 5, 8, 13." sqref="I2:I507">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Estimates Error!" error="Enter Story Points in Fibonacci!!!" promptTitle="Enter Story Points in Fibonacci" prompt="Enter Story Points in Fibonacci Series: 1, 2, 3, 5, 8, 13." sqref="I2:I506">
       <formula1>"1,2,3,5,8,13"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Status Error!" error="Please select Status only from the dropdown!!!" sqref="L2:L507">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Status Error!" error="Please select Status only from the dropdown!!!" sqref="L2:L506">
       <formula1>"Initial,Scheduled,WIP,Done"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>